<commit_message>
2021.11.24 Steady study. In constant study
</commit_message>
<xml_diff>
--- a/ExcelData_Tutorial/data/ch07/webpage_data/네이버_금융_환율_리스트.xlsx
+++ b/ExcelData_Tutorial/data/ch07/webpage_data/네이버_금융_환율_리스트.xlsx
@@ -558,19 +558,19 @@
         <v>7</v>
       </c>
       <c r="B2">
-        <v>1175</v>
+        <v>1187.9</v>
       </c>
       <c r="C2">
-        <v>1195.56</v>
+        <v>1208.68</v>
       </c>
       <c r="D2">
-        <v>1154.44</v>
+        <v>1167.12</v>
       </c>
       <c r="E2">
-        <v>1186.5</v>
+        <v>1199.5</v>
       </c>
       <c r="F2">
-        <v>1163.5</v>
+        <v>1176.3</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -581,22 +581,22 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>1367.52</v>
+        <v>1340.6</v>
       </c>
       <c r="C3">
-        <v>1394.73</v>
+        <v>1367.27</v>
       </c>
       <c r="D3">
-        <v>1340.31</v>
+        <v>1313.93</v>
       </c>
       <c r="E3">
-        <v>1381.19</v>
+        <v>1354</v>
       </c>
       <c r="F3">
-        <v>1353.85</v>
+        <v>1327.2</v>
       </c>
       <c r="G3">
-        <v>1.164</v>
+        <v>1.129</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -604,22 +604,22 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>1114.64</v>
+        <v>1040.69</v>
       </c>
       <c r="C4">
-        <v>1134.14</v>
+        <v>1058.9</v>
       </c>
       <c r="D4">
-        <v>1095.14</v>
+        <v>1022.48</v>
       </c>
       <c r="E4">
-        <v>1125.56</v>
+        <v>1050.88</v>
       </c>
       <c r="F4">
-        <v>1103.72</v>
+        <v>1030.5</v>
       </c>
       <c r="G4">
-        <v>0.9490000000000001</v>
+        <v>0.876</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -627,22 +627,22 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>171.69</v>
+        <v>185.88</v>
       </c>
       <c r="C5">
-        <v>180.27</v>
+        <v>195.17</v>
       </c>
       <c r="D5">
-        <v>163.11</v>
+        <v>176.59</v>
       </c>
       <c r="E5">
-        <v>173.4</v>
+        <v>187.73</v>
       </c>
       <c r="F5">
-        <v>169.98</v>
+        <v>184.03</v>
       </c>
       <c r="G5">
-        <v>0.146</v>
+        <v>0.157</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -650,22 +650,22 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>151.61</v>
+        <v>152.48</v>
       </c>
       <c r="C6">
-        <v>154.59</v>
+        <v>155.48</v>
       </c>
       <c r="D6">
-        <v>148.63</v>
+        <v>149.48</v>
       </c>
       <c r="E6">
-        <v>153.12</v>
+        <v>154</v>
       </c>
       <c r="F6">
-        <v>150.1</v>
+        <v>150.96</v>
       </c>
       <c r="G6">
-        <v>0.129</v>
+        <v>0.128</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -673,13 +673,13 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>40.13</v>
+        <v>42.72</v>
       </c>
       <c r="C7">
-        <v>45.38</v>
+        <v>48.31</v>
       </c>
       <c r="D7">
-        <v>37.33</v>
+        <v>39.73</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -688,7 +688,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0.034</v>
+        <v>0.036</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -696,22 +696,22 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>1492.13</v>
+        <v>1596.83</v>
       </c>
       <c r="C8">
-        <v>1521.52</v>
+        <v>1628.28</v>
       </c>
       <c r="D8">
-        <v>1462.74</v>
+        <v>1565.38</v>
       </c>
       <c r="E8">
-        <v>1507.05</v>
+        <v>1612.79</v>
       </c>
       <c r="F8">
-        <v>1477.21</v>
+        <v>1580.87</v>
       </c>
       <c r="G8">
-        <v>1.27</v>
+        <v>1.344</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -719,13 +719,13 @@
         <v>14</v>
       </c>
       <c r="B9">
-        <v>3051.95</v>
+        <v>3085.53</v>
       </c>
       <c r="C9">
-        <v>3323.57</v>
+        <v>3360.14</v>
       </c>
       <c r="D9">
-        <v>2868.84</v>
+        <v>2900.4</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -734,7 +734,7 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>2.597</v>
+        <v>2.598</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -742,22 +742,22 @@
         <v>15</v>
       </c>
       <c r="B10">
-        <v>877.78</v>
+        <v>939.5</v>
       </c>
       <c r="C10">
-        <v>895.0700000000001</v>
+        <v>958</v>
       </c>
       <c r="D10">
-        <v>860.49</v>
+        <v>921</v>
       </c>
       <c r="E10">
-        <v>886.55</v>
+        <v>948.89</v>
       </c>
       <c r="F10">
-        <v>869.01</v>
+        <v>930.11</v>
       </c>
       <c r="G10">
-        <v>0.747</v>
+        <v>0.791</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -765,22 +765,22 @@
         <v>16</v>
       </c>
       <c r="B11">
-        <v>1266.16</v>
+        <v>1278.76</v>
       </c>
       <c r="C11">
-        <v>1291.1</v>
+        <v>1303.95</v>
       </c>
       <c r="D11">
-        <v>1241.22</v>
+        <v>1253.57</v>
       </c>
       <c r="E11">
-        <v>1278.82</v>
+        <v>1291.54</v>
       </c>
       <c r="F11">
-        <v>1253.5</v>
+        <v>1265.98</v>
       </c>
       <c r="G11">
-        <v>1.078</v>
+        <v>1.077</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -788,22 +788,22 @@
         <v>17</v>
       </c>
       <c r="B12">
-        <v>128.31</v>
+        <v>132.76</v>
       </c>
       <c r="C12">
-        <v>131.45</v>
+        <v>136.01</v>
       </c>
       <c r="D12">
-        <v>125.17</v>
+        <v>129.51</v>
       </c>
       <c r="E12">
-        <v>129.59</v>
+        <v>134.08</v>
       </c>
       <c r="F12">
-        <v>127.03</v>
+        <v>131.44</v>
       </c>
       <c r="G12">
-        <v>0.109</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -811,22 +811,22 @@
         <v>18</v>
       </c>
       <c r="B13">
-        <v>826.14</v>
+        <v>859.6799999999999</v>
       </c>
       <c r="C13">
-        <v>842.41</v>
+        <v>876.61</v>
       </c>
       <c r="D13">
-        <v>809.87</v>
+        <v>842.75</v>
       </c>
       <c r="E13">
-        <v>834.4</v>
+        <v>868.27</v>
       </c>
       <c r="F13">
-        <v>817.88</v>
+        <v>851.09</v>
       </c>
       <c r="G13">
-        <v>0.703</v>
+        <v>0.724</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -834,22 +834,22 @@
         <v>19</v>
       </c>
       <c r="B14">
-        <v>769.27</v>
+        <v>831.17</v>
       </c>
       <c r="C14">
-        <v>784.42</v>
+        <v>847.54</v>
       </c>
       <c r="D14">
-        <v>754.12</v>
+        <v>814.8</v>
       </c>
       <c r="E14">
-        <v>776.96</v>
+        <v>839.48</v>
       </c>
       <c r="F14">
-        <v>761.58</v>
+        <v>822.86</v>
       </c>
       <c r="G14">
-        <v>0.655</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -857,22 +857,22 @@
         <v>20</v>
       </c>
       <c r="B15">
-        <v>50.42</v>
+        <v>52.75</v>
       </c>
       <c r="C15">
-        <v>54.7</v>
+        <v>57.23</v>
       </c>
       <c r="D15">
-        <v>45.89</v>
+        <v>48.01</v>
       </c>
       <c r="E15">
-        <v>50.97</v>
+        <v>53.33</v>
       </c>
       <c r="F15">
-        <v>49.87</v>
+        <v>52.17</v>
       </c>
       <c r="G15">
-        <v>0.043</v>
+        <v>0.044</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -880,13 +880,13 @@
         <v>21</v>
       </c>
       <c r="B16">
-        <v>1.5</v>
+        <v>1.43</v>
       </c>
       <c r="C16">
-        <v>1.62</v>
+        <v>1.54</v>
       </c>
       <c r="D16">
-        <v>1.38</v>
+        <v>1.32</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -903,7 +903,7 @@
         <v>22</v>
       </c>
       <c r="B17">
-        <v>154.27</v>
+        <v>106.16</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -912,13 +912,13 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>155.96</v>
+        <v>107.32</v>
       </c>
       <c r="F17">
-        <v>152.58</v>
+        <v>105</v>
       </c>
       <c r="G17">
-        <v>0.131</v>
+        <v>0.089</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -926,7 +926,7 @@
         <v>23</v>
       </c>
       <c r="B18">
-        <v>0.41</v>
+        <v>0.42</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -949,13 +949,13 @@
         <v>24</v>
       </c>
       <c r="B19">
-        <v>337.49</v>
+        <v>383.64</v>
       </c>
       <c r="C19">
-        <v>371.23</v>
+        <v>422</v>
       </c>
       <c r="D19">
-        <v>310.5</v>
+        <v>352.95</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -964,7 +964,7 @@
         <v>0</v>
       </c>
       <c r="G19">
-        <v>0.287</v>
+        <v>0.323</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -972,22 +972,22 @@
         <v>25</v>
       </c>
       <c r="B20">
-        <v>183.62</v>
+        <v>180.27</v>
       </c>
       <c r="C20">
-        <v>188.11</v>
+        <v>184.68</v>
       </c>
       <c r="D20">
-        <v>179.13</v>
+        <v>175.86</v>
       </c>
       <c r="E20">
-        <v>185.45</v>
+        <v>182.07</v>
       </c>
       <c r="F20">
-        <v>181.79</v>
+        <v>178.47</v>
       </c>
       <c r="G20">
-        <v>0.156</v>
+        <v>0.152</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -995,22 +995,22 @@
         <v>26</v>
       </c>
       <c r="B21">
-        <v>122.33</v>
+        <v>133.24</v>
       </c>
       <c r="C21">
-        <v>125.32</v>
+        <v>136.5</v>
       </c>
       <c r="D21">
-        <v>119.34</v>
+        <v>129.98</v>
       </c>
       <c r="E21">
-        <v>123.55</v>
+        <v>134.57</v>
       </c>
       <c r="F21">
-        <v>121.11</v>
+        <v>131.91</v>
       </c>
       <c r="G21">
-        <v>0.104</v>
+        <v>0.112</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1018,19 +1018,19 @@
         <v>27</v>
       </c>
       <c r="B22">
-        <v>313.27</v>
+        <v>316.68</v>
       </c>
       <c r="C22">
-        <v>333</v>
+        <v>336.63</v>
       </c>
       <c r="D22">
-        <v>291.66</v>
+        <v>294.83</v>
       </c>
       <c r="E22">
-        <v>316.4</v>
+        <v>319.84</v>
       </c>
       <c r="F22">
-        <v>310.14</v>
+        <v>313.52</v>
       </c>
       <c r="G22">
         <v>0.267</v>
@@ -1041,22 +1041,22 @@
         <v>28</v>
       </c>
       <c r="B23">
-        <v>3834.48</v>
+        <v>3926.29</v>
       </c>
       <c r="C23">
-        <v>4083.72</v>
+        <v>4181.49</v>
       </c>
       <c r="D23">
-        <v>3527.73</v>
+        <v>3612.19</v>
       </c>
       <c r="E23">
-        <v>3872.82</v>
+        <v>3965.55</v>
       </c>
       <c r="F23">
-        <v>3796.14</v>
+        <v>3887.03</v>
       </c>
       <c r="G23">
-        <v>3.263</v>
+        <v>3.305</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1064,22 +1064,22 @@
         <v>29</v>
       </c>
       <c r="B24">
-        <v>3115.88</v>
+        <v>3150.93</v>
       </c>
       <c r="C24">
-        <v>3315.29</v>
+        <v>3352.58</v>
       </c>
       <c r="D24">
-        <v>2866.61</v>
+        <v>2898.86</v>
       </c>
       <c r="E24">
-        <v>3147.03</v>
+        <v>3182.43</v>
       </c>
       <c r="F24">
-        <v>3084.73</v>
+        <v>3119.43</v>
       </c>
       <c r="G24">
-        <v>2.652</v>
+        <v>2.653</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1087,19 +1087,19 @@
         <v>30</v>
       </c>
       <c r="B25">
-        <v>319.89</v>
+        <v>323.41</v>
       </c>
       <c r="C25">
-        <v>337.48</v>
+        <v>341.19</v>
       </c>
       <c r="D25">
-        <v>297.82</v>
+        <v>301.1</v>
       </c>
       <c r="E25">
-        <v>323.08</v>
+        <v>326.64</v>
       </c>
       <c r="F25">
-        <v>316.7</v>
+        <v>320.18</v>
       </c>
       <c r="G25">
         <v>0.272</v>
@@ -1110,13 +1110,13 @@
         <v>31</v>
       </c>
       <c r="B26">
-        <v>1657.26</v>
+        <v>1677.23</v>
       </c>
       <c r="C26">
-        <v>1804.75</v>
+        <v>1826.5</v>
       </c>
       <c r="D26">
-        <v>1524.68</v>
+        <v>1543.06</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -1125,7 +1125,7 @@
         <v>0</v>
       </c>
       <c r="G26">
-        <v>1.41</v>
+        <v>1.412</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1133,7 +1133,7 @@
         <v>32</v>
       </c>
       <c r="B27">
-        <v>74.48</v>
+        <v>75.66</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1148,7 +1148,7 @@
         <v>0</v>
       </c>
       <c r="G27">
-        <v>0.063</v>
+        <v>0.064</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1156,22 +1156,22 @@
         <v>33</v>
       </c>
       <c r="B28">
-        <v>37.12</v>
+        <v>36.17</v>
       </c>
       <c r="C28">
-        <v>38.97</v>
+        <v>37.97</v>
       </c>
       <c r="D28">
-        <v>34.9</v>
+        <v>34</v>
       </c>
       <c r="E28">
-        <v>37.49</v>
+        <v>36.53</v>
       </c>
       <c r="F28">
-        <v>36.75</v>
+        <v>35.81</v>
       </c>
       <c r="G28">
-        <v>0.032</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1179,22 +1179,22 @@
         <v>34</v>
       </c>
       <c r="B29">
-        <v>852.62</v>
+        <v>871.95</v>
       </c>
       <c r="C29">
-        <v>869.58</v>
+        <v>889.3</v>
       </c>
       <c r="D29">
-        <v>835.66</v>
+        <v>854.6</v>
       </c>
       <c r="E29">
-        <v>861.14</v>
+        <v>880.66</v>
       </c>
       <c r="F29">
-        <v>844.1</v>
+        <v>863.24</v>
       </c>
       <c r="G29">
-        <v>0.726</v>
+        <v>0.734</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1202,22 +1202,22 @@
         <v>35</v>
       </c>
       <c r="B30">
-        <v>281.94</v>
+        <v>283.64</v>
       </c>
       <c r="C30">
-        <v>299.7</v>
+        <v>301.5</v>
       </c>
       <c r="D30">
-        <v>261.08</v>
+        <v>262.66</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
       <c r="F30">
-        <v>279.13</v>
+        <v>280.81</v>
       </c>
       <c r="G30">
-        <v>0.24</v>
+        <v>0.239</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -1225,22 +1225,22 @@
         <v>36</v>
       </c>
       <c r="B31">
-        <v>7.93</v>
+        <v>8.359999999999999</v>
       </c>
       <c r="C31">
-        <v>8.48</v>
+        <v>8.94</v>
       </c>
       <c r="D31">
-        <v>7.14</v>
+        <v>7.53</v>
       </c>
       <c r="E31">
-        <v>8</v>
+        <v>8.44</v>
       </c>
       <c r="F31">
-        <v>7.86</v>
+        <v>8.279999999999999</v>
       </c>
       <c r="G31">
-        <v>0.006999999999999999</v>
+        <v>0.007</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1248,7 +1248,7 @@
         <v>37</v>
       </c>
       <c r="B32">
-        <v>322.65</v>
+        <v>324.3</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -1263,7 +1263,7 @@
         <v>0</v>
       </c>
       <c r="G32">
-        <v>0.275</v>
+        <v>0.273</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1271,7 +1271,7 @@
         <v>38</v>
       </c>
       <c r="B33">
-        <v>2.75</v>
+        <v>2.74</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -1294,13 +1294,13 @@
         <v>39</v>
       </c>
       <c r="B34">
-        <v>852.62</v>
+        <v>871.95</v>
       </c>
       <c r="C34">
-        <v>886.72</v>
+        <v>906.8200000000001</v>
       </c>
       <c r="D34">
-        <v>801.47</v>
+        <v>819.64</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -1309,7 +1309,7 @@
         <v>0</v>
       </c>
       <c r="G34">
-        <v>0.726</v>
+        <v>0.734</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -1317,7 +1317,7 @@
         <v>40</v>
       </c>
       <c r="B35">
-        <v>15.94</v>
+        <v>15.98</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -1340,7 +1340,7 @@
         <v>41</v>
       </c>
       <c r="B36">
-        <v>7.09</v>
+        <v>6.79</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -1363,7 +1363,7 @@
         <v>42</v>
       </c>
       <c r="B37">
-        <v>13.86</v>
+        <v>13.85</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -1386,22 +1386,22 @@
         <v>43</v>
       </c>
       <c r="B38">
-        <v>24.22</v>
+        <v>23.41</v>
       </c>
       <c r="C38">
-        <v>26.64</v>
+        <v>25.75</v>
       </c>
       <c r="D38">
-        <v>22.24</v>
+        <v>21.5</v>
       </c>
       <c r="E38">
-        <v>24.46</v>
+        <v>23.64</v>
       </c>
       <c r="F38">
-        <v>23.98</v>
+        <v>23.18</v>
       </c>
       <c r="G38">
-        <v>0.021</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -1409,22 +1409,22 @@
         <v>44</v>
       </c>
       <c r="B39">
-        <v>52.51</v>
+        <v>56.98</v>
       </c>
       <c r="C39">
-        <v>57.76</v>
+        <v>62.67</v>
       </c>
       <c r="D39">
-        <v>48.1</v>
+        <v>52.2</v>
       </c>
       <c r="E39">
-        <v>53.03</v>
+        <v>57.54</v>
       </c>
       <c r="F39">
-        <v>51.99</v>
+        <v>56.42</v>
       </c>
       <c r="G39">
-        <v>0.045</v>
+        <v>0.048</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -1432,22 +1432,22 @@
         <v>45</v>
       </c>
       <c r="B40">
-        <v>213.25</v>
+        <v>211.61</v>
       </c>
       <c r="C40">
-        <v>235</v>
+        <v>233.19</v>
       </c>
       <c r="D40">
-        <v>196.19</v>
+        <v>194.69</v>
       </c>
       <c r="E40">
         <v>0</v>
       </c>
       <c r="F40">
-        <v>210.7</v>
+        <v>209.08</v>
       </c>
       <c r="G40">
-        <v>0.182</v>
+        <v>0.178</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1455,19 +1455,19 @@
         <v>46</v>
       </c>
       <c r="B41">
-        <v>5.07</v>
+        <v>5.24</v>
       </c>
       <c r="C41">
-        <v>5.66</v>
+        <v>5.85</v>
       </c>
       <c r="D41">
-        <v>4.48</v>
+        <v>4.63</v>
       </c>
       <c r="E41">
-        <v>5.12</v>
+        <v>5.29</v>
       </c>
       <c r="F41">
-        <v>5.02</v>
+        <v>5.19</v>
       </c>
       <c r="G41">
         <v>0.004</v>
@@ -1478,22 +1478,22 @@
         <v>47</v>
       </c>
       <c r="B42">
-        <v>68.55</v>
+        <v>75.45</v>
       </c>
       <c r="C42">
-        <v>72.66</v>
+        <v>79.97</v>
       </c>
       <c r="D42">
-        <v>63.07</v>
+        <v>69.42</v>
       </c>
       <c r="E42">
-        <v>69.37</v>
+        <v>76.34999999999999</v>
       </c>
       <c r="F42">
-        <v>67.73</v>
+        <v>74.55</v>
       </c>
       <c r="G42">
-        <v>0.058</v>
+        <v>0.064</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -1501,22 +1501,22 @@
         <v>48</v>
       </c>
       <c r="B43">
-        <v>15.12</v>
+        <v>16.16</v>
       </c>
       <c r="C43">
-        <v>16.17</v>
+        <v>17.29</v>
       </c>
       <c r="D43">
-        <v>13.46</v>
+        <v>14.39</v>
       </c>
       <c r="E43">
-        <v>15.27</v>
+        <v>16.32</v>
       </c>
       <c r="F43">
-        <v>14.97</v>
+        <v>16</v>
       </c>
       <c r="G43">
-        <v>0.013</v>
+        <v>0.014</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -1524,19 +1524,19 @@
         <v>49</v>
       </c>
       <c r="B44">
-        <v>3.76</v>
+        <v>3.65</v>
       </c>
       <c r="C44">
-        <v>4.1</v>
+        <v>3.98</v>
       </c>
       <c r="D44">
-        <v>3.46</v>
+        <v>3.36</v>
       </c>
       <c r="E44">
-        <v>3.8</v>
+        <v>3.69</v>
       </c>
       <c r="F44">
-        <v>3.72</v>
+        <v>3.61</v>
       </c>
       <c r="G44">
         <v>0.003</v>
@@ -1547,22 +1547,22 @@
         <v>50</v>
       </c>
       <c r="B45">
-        <v>299.84</v>
+        <v>285.72</v>
       </c>
       <c r="C45">
-        <v>323.82</v>
+        <v>308.57</v>
       </c>
       <c r="D45">
-        <v>275.86</v>
+        <v>262.87</v>
       </c>
       <c r="E45">
-        <v>303.13</v>
+        <v>288.86</v>
       </c>
       <c r="F45">
-        <v>296.55</v>
+        <v>282.58</v>
       </c>
       <c r="G45">
-        <v>0.255</v>
+        <v>0.241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>